<commit_message>
Updated T8 with correct structure
</commit_message>
<xml_diff>
--- a/data/excel/T8.xlsx
+++ b/data/excel/T8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Downloads\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\GitHub\Data-Visualisation-2\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B59CACDD-54AD-4D61-96BD-B8AD64875F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2D3CB9-51E2-4C7B-822A-358119F473AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{50F6FE6F-C46E-48C6-B8D9-EE964304E308}"/>
   </bookViews>
@@ -449,21 +449,21 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -471,112 +471,112 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>7.662071835686592</v>
+        <v>40.595240908339044</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>4.803777738814647</v>
+        <v>59.404759091660949</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4">
-        <v>28.554564163774863</v>
+        <v>69.725076873280472</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>17.036577924574008</v>
+        <v>30.274923126719532</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6">
-        <v>41.943008337149898</v>
+        <v>56.997482795765933</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7">
-        <v>19.468388770508366</v>
+        <v>43.002517204234067</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>3.6217179655651832</v>
+        <v>63.171383255322155</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
       <c r="C9">
-        <v>37.406873653093847</v>
+        <v>36.828616744677845</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>17.245868076100727</v>
+        <v>76.592353688848576</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
       <c r="C11">
-        <v>22.257151534731879</v>
+        <v>23.407646311151431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>